<commit_message>
varie prove su plot
</commit_message>
<xml_diff>
--- a/src/plot/data.xlsx
+++ b/src/plot/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmg\C++\repos\pv-creativity\src\plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B036C2-CE75-4738-8052-45E0C8C79E5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBDBCD9-49CA-471A-9EC0-AFF19C9D5104}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{1D304B6E-3250-49F2-8804-68E9AF85D498}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{1D304B6E-3250-49F2-8804-68E9AF85D498}"/>
   </bookViews>
   <sheets>
     <sheet name="Irradiance" sheetId="1" r:id="rId1"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Irradiance 10" sheetId="3" r:id="rId2"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>G</t>
   </si>
@@ -397,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD275-E1D7-4EEB-BD3F-3DAD75B36FEF}">
   <dimension ref="A1:P367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="X45" sqref="X45"/>
     </sheetView>
   </sheetViews>
@@ -561,7 +562,7 @@
         <v>0.60688534246233383</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:L67" si="2">$B$1*C$2*$B4</f>
+        <f t="shared" ref="C4:L42" si="2">$B$1*C$2*$B4</f>
         <v>400.54432602514026</v>
       </c>
       <c r="D4">
@@ -2472,7 +2473,7 @@
         <v>0.73824492506829331</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:L106" si="3">$B$1*C$2*$B43</f>
+        <f t="shared" ref="C43:L68" si="3">$B$1*C$2*$B43</f>
         <v>487.24165054507353</v>
       </c>
       <c r="D43">
@@ -3717,7 +3718,7 @@
         <v>978.24248233838387</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="D68:L131" si="5">$B$1*H$2*$B68</f>
+        <f t="shared" ref="D68:L96" si="5">$B$1*H$2*$B68</f>
         <v>831.50610998762625</v>
       </c>
       <c r="I68">
@@ -5101,7 +5102,7 @@
         <v>587.04202611012067</v>
       </c>
       <c r="K96">
-        <f t="shared" ref="D96:L159" si="7">$B$1*K$2*$B96</f>
+        <f t="shared" ref="D96:L125" si="7">$B$1*K$2*$B96</f>
         <v>426.93965535281501</v>
       </c>
       <c r="L96">
@@ -6498,7 +6499,7 @@
         <v>796.89332308633209</v>
       </c>
       <c r="E125">
-        <f t="shared" ref="D125:L188" si="8">$B$1*E$2*$B125</f>
+        <f t="shared" ref="D125:L153" si="8">$B$1*E$2*$B125</f>
         <v>967.65617803340331</v>
       </c>
       <c r="F125">
@@ -7882,7 +7883,7 @@
         <v>1182.4658633107915</v>
       </c>
       <c r="H153">
-        <f t="shared" ref="D153:L216" si="11">$B$1*H$2*$B153</f>
+        <f t="shared" ref="D153:L181" si="11">$B$1*H$2*$B153</f>
         <v>1005.0959838141728</v>
       </c>
       <c r="I153">
@@ -9266,7 +9267,7 @@
         <v>659.88021810146222</v>
       </c>
       <c r="K181">
-        <f t="shared" ref="D181:L244" si="12">$B$1*K$2*$B181</f>
+        <f t="shared" ref="D181:L210" si="12">$B$1*K$2*$B181</f>
         <v>479.91288589197245</v>
       </c>
       <c r="L181">
@@ -10663,7 +10664,7 @@
         <v>831.93954501247572</v>
       </c>
       <c r="E210">
-        <f t="shared" ref="D210:L273" si="15">$B$1*E$2*$B210</f>
+        <f t="shared" ref="D210:L238" si="15">$B$1*E$2*$B210</f>
         <v>1010.2123046580062</v>
       </c>
       <c r="F210">
@@ -12047,7 +12048,7 @@
         <v>1150.0028595527563</v>
       </c>
       <c r="H238">
-        <f t="shared" ref="D238:L301" si="16">$B$1*H$2*$B238</f>
+        <f t="shared" ref="D238:L266" si="16">$B$1*H$2*$B238</f>
         <v>977.50243061984293</v>
       </c>
       <c r="I238">
@@ -13431,7 +13432,7 @@
         <v>597.66659377670317</v>
       </c>
       <c r="K266">
-        <f t="shared" ref="D266:L329" si="19">$B$1*K$2*$B266</f>
+        <f t="shared" ref="D266:L295" si="19">$B$1*K$2*$B266</f>
         <v>434.66661365578409</v>
       </c>
       <c r="L266">
@@ -14828,7 +14829,7 @@
         <v>699.14889188047709</v>
       </c>
       <c r="E295">
-        <f t="shared" ref="D295:L358" si="20">$B$1*E$2*$B295</f>
+        <f t="shared" ref="D295:L323" si="20">$B$1*E$2*$B295</f>
         <v>848.96651156915073</v>
       </c>
       <c r="F295">
@@ -16212,7 +16213,7 @@
         <v>897.46778058752307</v>
       </c>
       <c r="H323">
-        <f t="shared" ref="D323:L367" si="21">$B$1*H$2*$B323</f>
+        <f t="shared" ref="D323:L351" si="21">$B$1*H$2*$B323</f>
         <v>762.84761349939458</v>
       </c>
       <c r="I323">
@@ -18394,6 +18395,1968 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD35DC7-E27E-4586-A7CE-FA7E0AECE9CE}">
+  <dimension ref="A1:P39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1200</v>
+      </c>
+      <c r="C1">
+        <v>9</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>11</v>
+      </c>
+      <c r="F1">
+        <v>12</v>
+      </c>
+      <c r="G1">
+        <v>13</v>
+      </c>
+      <c r="H1">
+        <v>14</v>
+      </c>
+      <c r="I1">
+        <v>15</v>
+      </c>
+      <c r="J1">
+        <v>16</v>
+      </c>
+      <c r="K1">
+        <v>17</v>
+      </c>
+      <c r="L1">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <f>MAX(C3:L367)</f>
+        <v>1199.8888809503476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>D2-0.15</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="D2">
+        <f>E2-0.15</f>
+        <v>0.7</v>
+      </c>
+      <c r="E2">
+        <f>F2-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="F2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>G2-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="I2">
+        <f>H2-0.15</f>
+        <v>0.7</v>
+      </c>
+      <c r="J2">
+        <f>I2-0.15</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="K2">
+        <f>J2-0.15</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="L2">
+        <f>K2-0.15</f>
+        <v>0.24999999999999992</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <f>MAX(B3:B367)</f>
+        <v>0.99990740079195639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>SIN(A3/365*PI())*0.4+0.6</f>
+        <v>0.60344279875547535</v>
+      </c>
+      <c r="C3">
+        <f>$B$1*C$2*$B3</f>
+        <v>398.27224717861367</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:L18" si="0">$B$1*D$2*$B3</f>
+        <v>506.89195095459928</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>615.51165473058484</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>724.13135850657045</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>724.13135850657045</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>615.51165473058484</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>506.89195095459928</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>398.27224717861367</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>289.65254340262811</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>181.03283962664253</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <f>MIN(C3:L367)</f>
+        <v>181.03283962664253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B67" si="1">SIN(A4/365*PI())*0.4+0.6</f>
+        <v>0.63438591949497858</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:L42" si="2">$B$1*C$2*$B4</f>
+        <v>418.69470686668581</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>532.88417237578199</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>647.07363788487817</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>761.26310339397435</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>761.26310339397435</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>647.07363788487817</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>532.88417237578199</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>418.69470686668581</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>304.50524135758963</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>190.3157758484935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>0.66851725767259107</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>441.22139006391001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>561.55449644497651</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>681.88760282604289</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>802.22070920710928</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>802.22070920710928</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>681.88760282604289</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>561.55449644497651</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>441.22139006391001</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>320.88828368284362</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>200.55517730177723</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+10</f>
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>0.70214131804647484</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>463.41326991067331</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>589.79870715903883</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>716.18414440740435</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>842.56958165576975</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>842.56958165576975</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>716.18414440740435</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>589.79870715903883</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>463.41326991067331</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>337.02783266230784</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>210.64239541394238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7:A59" si="3">A6+10</f>
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0.73500915983764536</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>485.10604549284585</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>617.40769426362215</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>749.70934303439822</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>882.0109918051744</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>882.0109918051744</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>749.70934303439822</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>617.40769426362215</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>485.10604549284585</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>352.80439672206967</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>220.50274795129351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>0.76687744104492672</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>506.13911108965152</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>644.17705047773848</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>782.21498986582526</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>920.25292925391204</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>920.25292925391204</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>782.21498986582526</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>644.17705047773848</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>506.13911108965152</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>368.10117170156474</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>230.06323231347793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>0.79751022006399086</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>526.35674524223384</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>669.90858485375236</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>813.46042446527065</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>957.01226407678905</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>957.01226407678905</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>813.46042446527065</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>669.90858485375236</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>526.35674524223384</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>382.8049056307155</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>239.25306601919718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>0.82668070251644699</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>545.60926366085494</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>694.41179011381541</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>843.21431656677589</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>992.01684301973637</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>992.01684301973637</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>843.21431656677589</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>694.41179011381541</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>545.60926366085494</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>396.80673720789446</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>248.00421075493401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>0.85417292035607095</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>563.75412743500669</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>717.5052530990996</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>871.2563787631924</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1025.0075044272851</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1025.0075044272851</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>871.2563787631924</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>717.5052530990996</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>563.75412743500669</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>410.00300177091395</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>256.25187610682121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>0.87978333082065885</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>580.65699834163479</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>739.01799788935341</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>897.37899743707203</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1055.7399969847907</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1055.7399969847907</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>897.37899743707203</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>739.01799788935341</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>580.65699834163479</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>422.29599879391617</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>263.93499924619755</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>0.90332232339142493</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>596.19273343834038</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>758.79075164879691</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>921.38876985925344</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1083.98678806971</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1083.98678806971</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>921.38876985925344</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>758.79075164879691</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>596.19273343834038</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>433.59471522788385</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>270.99669701742738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0.92461562360294436</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>610.24631157794317</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>776.67712382647323</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>943.10793607500329</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1109.5387483235331</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1109.5387483235331</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>943.10793607500329</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>776.67712382647323</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>610.24631157794317</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>443.81549932941317</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>277.38468708088323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>0.94350558331032119</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>622.71368498481183</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>792.54468998066977</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>962.3756949765276</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1132.2066999723854</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1132.2066999723854</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>962.3756949765276</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>792.54468998066977</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>622.71368498481183</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>452.88267998895407</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>283.05167499309624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0.95985234786089735</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>633.5025495881921</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>806.27597220315374</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>979.04939481811527</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1151.8228174330768</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1151.8228174330768</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>979.04939481811527</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>806.27597220315374</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>633.5025495881921</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>460.72912697323062</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>287.95570435826909</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0.97353489152917005</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>642.5330284092521</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>817.76930888450283</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>993.00558935975346</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1168.2418698350041</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1168.2418698350041</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>993.00558935975346</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>817.76930888450283</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>642.5330284092521</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>467.29674793400153</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>292.06046745875091</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.98445191354892025</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>649.73826294228729</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>826.93960738109297</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1004.1409518198986</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1181.3422962587042</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1181.3422962587042</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1004.1409518198986</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>826.93960738109297</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>649.73826294228729</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>472.53691850348162</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>295.33557406467594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0.99252258810864369</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>655.06490815170469</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>833.71897401126068</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1012.3730398708166</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>1191.0271057303723</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>1191.0271057303723</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>1012.3730398708166</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>833.71897401126068</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>655.06490815170469</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>476.41084229214886</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>297.75677643259297</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>0.99768716275758074</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>658.47352742000317</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>838.05721671636786</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1017.6409060127323</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>1197.2245953090969</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>1197.2245953090969</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>1017.6409060127323</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>838.05721671636786</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>658.47352742000317</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>478.88983812363864</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>299.30614882727411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>0.99990740079195639</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>659.93888452269107</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>839.92221666524335</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1019.9055488077955</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1199.8888809503476</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>1199.8888809503476</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>1019.9055488077955</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>839.92221666524335</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>659.93888452269107</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>479.95555238013895</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>299.97222023758678</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>0.99916686434615687</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>659.45013046846339</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>839.30016605077174</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1019.15020163308</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>1199.0002372153883</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>1199.0002372153883</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>1019.15020163308</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>839.30016605077174</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>659.45013046846339</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>479.6000948861552</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>299.75005930384697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>0.99547103609293619</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>657.01088382133776</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>836.19567031806639</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>1015.3804568147949</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>1194.5652433115233</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>1194.5652433115233</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>1015.3804568147949</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>836.19567031806639</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>657.01088382133776</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>477.82609732460924</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>298.64131082788072</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>0.98884727865162447</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>652.63920391007207</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>830.63171406736456</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>1008.6242242246569</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1186.6167343819493</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>1186.6167343819493</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>1008.6242242246569</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>830.63171406736456</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>652.63920391007207</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>474.64669375277964</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>296.65418359548721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>0.97934463200486865</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>646.36745712321317</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>822.64949088408969</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>998.93152464496598</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1175.2135584058424</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>1175.2135584058424</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>998.93152464496598</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>822.64949088408969</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>646.36745712321317</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>470.08542336233683</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>293.80338960146048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>0.96703345042375755</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>638.24207727967985</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>812.3080983559563</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>986.37411943223265</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>1160.4401405085091</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>1160.4401405085091</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>986.37411943223265</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>812.3080983559563</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>638.24207727967985</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>464.1760562034035</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>290.11003512712716</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>0.95200488158941432</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>628.32322184901329</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>799.68410053510797</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>971.04497922120265</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>1142.4058579072971</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>1142.4058579072971</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>971.04497922120265</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>799.68410053510797</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>628.32322184901329</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>456.96234316291878</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>285.60146447682416</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>0.93437019176745484</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>616.6843265665201</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>784.8709610846621</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>953.05759560280399</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1121.2442301209458</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>1121.2442301209458</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>953.05759560280399</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>784.8709610846621</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>616.6843265665201</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="2"/>
+        <v>448.49769204837821</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>280.31105753023633</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>260</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>0.91425994203148586</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>603.4115617407806</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>767.97835130644808</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>932.54514087211555</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1097.111930437783</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>1097.111930437783</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>932.54514087211555</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>767.97835130644808</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>603.4115617407806</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>438.84477217511312</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>274.27798260944564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>0.89182302163459504</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>588.60319427883258</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>749.13133817305982</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>909.65948206728694</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>1070.187625961514</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>1070.187625961514</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>909.65948206728694</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>749.13133817305982</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>588.60319427883258</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="2"/>
+        <v>428.0750503846055</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>267.54690649037843</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>0.86722554568541343</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>572.3688601523728</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>728.46945837574731</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>884.5700565991217</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1040.6706548224961</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>1040.6706548224961</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>884.5700565991217</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>728.46945837574731</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>572.3688601523728</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
+        <v>416.26826192899836</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>260.16766370562391</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>290</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>0.84064962528996912</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>554.82875269137958</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>706.14568524357401</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>857.46261779576855</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>1008.779550347963</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>1008.779550347963</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>857.46261779576855</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>706.14568524357401</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>554.82875269137958</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="2"/>
+        <v>403.51182013918509</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>252.19488758699063</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>0.81229201926477346</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>536.11273271475034</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>682.32529618240972</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>828.53785965006898</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>974.75042311772813</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>974.75042311772813</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>828.53785965006898</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>682.32529618240972</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>536.11273271475034</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="2"/>
+        <v>389.90016924709118</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>243.68760577943195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>310</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>0.7823626774033835</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>516.35936708623296</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>657.18464901884215</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>798.00993095145122</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>938.83521288406018</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>938.83521288406018</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>798.00993095145122</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>657.18464901884215</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>516.35936708623296</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>375.53408515362401</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>234.70880322101496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>0.75108318608158597</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>495.71490281384666</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>630.90987630853226</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>766.10484980321769</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>901.29982329790312</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>901.29982329790312</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>766.10484980321769</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>630.90987630853226</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>495.71490281384666</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="2"/>
+        <v>360.51992931916118</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>225.32495582447569</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>330</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>0.71868512770939608</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>474.33218428820135</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>603.69550727589274</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>733.05883026358401</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>862.42215325127529</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>862.42215325127529</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>733.05883026358401</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>603.69550727589274</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>474.33218428820135</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="2"/>
+        <v>344.96886130051001</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>215.60553831281874</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>0.68540836617591849</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>452.3695216761061</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>575.74302758777151</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>699.11653349943685</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>822.4900394111022</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>822.4900394111022</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>699.11653349943685</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>575.74302758777151</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>452.3695216761061</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>328.99601576444081</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>205.62250985277547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>0.65149927098103233</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>429.98951884748124</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>547.25938762406713</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>664.52925640065303</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>781.79912517723881</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>781.79912517723881</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>664.52925640065303</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>547.25938762406713</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>429.98951884748124</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>312.71965007089545</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>195.44978129430962</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>0.61720889320181227</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>407.35786951319602</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>518.45547028952228</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>629.55307106584848</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>740.65067184217469</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>740.65067184217469</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>629.55307106584848</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>518.45547028952228</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>407.35786951319602</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="2"/>
+        <v>296.26026873686982</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>185.16266796054362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CF1ADD-2FEC-408D-894C-6403C71ADEB4}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>